<commit_message>
Refactoring the codes and adding the docstrings
</commit_message>
<xml_diff>
--- a/output/Arctic_Bay/k_3/clusters_data.xlsx
+++ b/output/Arctic_Bay/k_3/clusters_data.xlsx
@@ -38,42 +38,186 @@
     <t>1001</t>
   </si>
   <si>
+    <t>181</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
     <t>23</t>
   </si>
   <si>
+    <t>155</t>
+  </si>
+  <si>
     <t>1013</t>
   </si>
   <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
     <t>1014</t>
   </si>
   <si>
+    <t>186</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>183</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
     <t>91</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
     <t>77</t>
   </si>
   <si>
+    <t>153</t>
+  </si>
+  <si>
     <t>50</t>
   </si>
   <si>
     <t>94</t>
   </si>
   <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
     <t>79</t>
   </si>
   <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
     <t>52</t>
   </si>
   <si>
     <t>132</t>
   </si>
   <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
     <t>138</t>
   </si>
   <si>
     <t>1012</t>
   </si>
   <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
     <t>96</t>
   </si>
   <si>
@@ -101,6 +245,12 @@
     <t>135</t>
   </si>
   <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
     <t>53</t>
   </si>
   <si>
@@ -113,18 +263,39 @@
     <t>93</t>
   </si>
   <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
     <t>95</t>
   </si>
   <si>
     <t>139</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>99</t>
   </si>
   <si>
+    <t>17</t>
+  </si>
+  <si>
     <t>92</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>101</t>
   </si>
   <si>
@@ -140,6 +311,9 @@
     <t>130</t>
   </si>
   <si>
+    <t>104</t>
+  </si>
+  <si>
     <t>27</t>
   </si>
   <si>
@@ -209,6 +383,69 @@
     <t>28</t>
   </si>
   <si>
+    <t>209</t>
+  </si>
+  <si>
+    <t>218</t>
+  </si>
+  <si>
+    <t>217</t>
+  </si>
+  <si>
+    <t>216</t>
+  </si>
+  <si>
+    <t>334</t>
+  </si>
+  <si>
+    <t>220</t>
+  </si>
+  <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>206</t>
+  </si>
+  <si>
+    <t>208</t>
+  </si>
+  <si>
+    <t>203</t>
+  </si>
+  <si>
+    <t>204</t>
+  </si>
+  <si>
+    <t>202</t>
+  </si>
+  <si>
+    <t>212</t>
+  </si>
+  <si>
+    <t>214</t>
+  </si>
+  <si>
+    <t>215</t>
+  </si>
+  <si>
+    <t>219</t>
+  </si>
+  <si>
+    <t>213</t>
+  </si>
+  <si>
+    <t>205</t>
+  </si>
+  <si>
+    <t>211</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>177</t>
+  </si>
+  <si>
     <t>321</t>
   </si>
   <si>
@@ -227,27 +464,18 @@
     <t>291</t>
   </si>
   <si>
-    <t>209</t>
-  </si>
-  <si>
-    <t>218</t>
-  </si>
-  <si>
-    <t>217</t>
-  </si>
-  <si>
-    <t>216</t>
-  </si>
-  <si>
-    <t>334</t>
-  </si>
-  <si>
     <t>316</t>
   </si>
   <si>
     <t>280</t>
   </si>
   <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
     <t>312</t>
   </si>
   <si>
@@ -275,6 +503,9 @@
     <t>306</t>
   </si>
   <si>
+    <t>187</t>
+  </si>
+  <si>
     <t>296</t>
   </si>
   <si>
@@ -290,9 +521,18 @@
     <t>292</t>
   </si>
   <si>
+    <t>193</t>
+  </si>
+  <si>
+    <t>173</t>
+  </si>
+  <si>
     <t>294</t>
   </si>
   <si>
+    <t>170</t>
+  </si>
+  <si>
     <t>315</t>
   </si>
   <si>
@@ -305,6 +545,15 @@
     <t>303</t>
   </si>
   <si>
+    <t>168</t>
+  </si>
+  <si>
+    <t>174</t>
+  </si>
+  <si>
+    <t>172</t>
+  </si>
+  <si>
     <t>313</t>
   </si>
   <si>
@@ -323,7 +572,10 @@
     <t>196</t>
   </si>
   <si>
-    <t>220</t>
+    <t>190</t>
+  </si>
+  <si>
+    <t>195</t>
   </si>
   <si>
     <t>201</t>
@@ -335,262 +587,10 @@
     <t>200</t>
   </si>
   <si>
-    <t>207</t>
-  </si>
-  <si>
-    <t>206</t>
-  </si>
-  <si>
-    <t>208</t>
-  </si>
-  <si>
     <t>323</t>
   </si>
   <si>
-    <t>203</t>
-  </si>
-  <si>
-    <t>204</t>
-  </si>
-  <si>
-    <t>202</t>
-  </si>
-  <si>
     <t>199</t>
-  </si>
-  <si>
-    <t>212</t>
-  </si>
-  <si>
-    <t>214</t>
-  </si>
-  <si>
-    <t>215</t>
-  </si>
-  <si>
-    <t>219</t>
-  </si>
-  <si>
-    <t>213</t>
-  </si>
-  <si>
-    <t>205</t>
-  </si>
-  <si>
-    <t>211</t>
-  </si>
-  <si>
-    <t>210</t>
-  </si>
-  <si>
-    <t>177</t>
-  </si>
-  <si>
-    <t>188</t>
-  </si>
-  <si>
-    <t>189</t>
-  </si>
-  <si>
-    <t>181</t>
-  </si>
-  <si>
-    <t>187</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>179</t>
-  </si>
-  <si>
-    <t>155</t>
-  </si>
-  <si>
-    <t>157</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>185</t>
-  </si>
-  <si>
-    <t>186</t>
-  </si>
-  <si>
-    <t>184</t>
-  </si>
-  <si>
-    <t>182</t>
-  </si>
-  <si>
-    <t>180</t>
-  </si>
-  <si>
-    <t>183</t>
-  </si>
-  <si>
-    <t>147</t>
-  </si>
-  <si>
-    <t>142</t>
-  </si>
-  <si>
-    <t>158</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>68</t>
-  </si>
-  <si>
-    <t>113</t>
-  </si>
-  <si>
-    <t>149</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>193</t>
-  </si>
-  <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>66</t>
-  </si>
-  <si>
-    <t>67</t>
-  </si>
-  <si>
-    <t>58</t>
-  </si>
-  <si>
-    <t>173</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>64</t>
-  </si>
-  <si>
-    <t>62</t>
-  </si>
-  <si>
-    <t>156</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>153</t>
-  </si>
-  <si>
-    <t>160</t>
-  </si>
-  <si>
-    <t>170</t>
-  </si>
-  <si>
-    <t>112</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>162</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
-    <t>114</t>
-  </si>
-  <si>
-    <t>168</t>
-  </si>
-  <si>
-    <t>116</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>69</t>
-  </si>
-  <si>
-    <t>174</t>
-  </si>
-  <si>
-    <t>172</t>
-  </si>
-  <si>
-    <t>115</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>143</t>
-  </si>
-  <si>
-    <t>141</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>61</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>145</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>190</t>
-  </si>
-  <si>
-    <t>195</t>
   </si>
 </sst>
 </file>
@@ -931,18 +931,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BW4"/>
+  <dimension ref="A1:ED4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:75">
+    <row r="1" spans="1:134">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:75">
+    <row r="2" spans="1:134">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -968,13 +968,13 @@
         <v>7</v>
       </c>
       <c r="I2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L2" t="s">
         <v>10</v>
@@ -1016,43 +1016,43 @@
         <v>22</v>
       </c>
       <c r="Y2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z2" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>34</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>27</v>
       </c>
       <c r="AL2" t="s">
         <v>35</v>
@@ -1067,502 +1067,502 @@
         <v>38</v>
       </c>
       <c r="AP2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>49</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>51</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>54</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>55</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>56</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>62</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>63</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>64</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>65</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>71</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>72</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>74</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>75</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>76</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>77</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>78</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>79</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>80</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>81</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>82</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>83</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>84</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>85</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>86</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>87</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>88</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>89</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>75</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>90</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>91</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>92</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>93</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>94</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>95</v>
+      </c>
+      <c r="CV2" t="s">
         <v>4</v>
       </c>
-      <c r="AQ2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AU2" t="s">
+      <c r="CW2" t="s">
+        <v>96</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>62</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>97</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>98</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>47</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>99</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>100</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>10</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>81</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>101</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>102</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>103</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>104</v>
+      </c>
+      <c r="DJ2" t="s">
         <v>41</v>
       </c>
-      <c r="AV2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>44</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>45</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>46</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>11</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>47</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>48</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>49</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>50</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>51</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>52</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>35</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>32</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>54</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>55</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>56</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>57</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>58</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>59</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>60</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>61</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>62</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>63</v>
+      <c r="DK2" t="s">
+        <v>105</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>106</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>107</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>70</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>108</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>109</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>110</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>91</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>111</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>86</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>112</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>113</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>114</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>115</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>116</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>117</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>118</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>119</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>120</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:75">
+    <row r="3" spans="1:134">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>128</v>
       </c>
       <c r="I3" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="J3" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="K3" t="s">
-        <v>73</v>
+        <v>131</v>
       </c>
       <c r="L3" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="M3" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
       <c r="N3" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="O3" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="P3" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="Q3" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="R3" t="s">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="S3" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="T3" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="U3" t="s">
-        <v>83</v>
-      </c>
-      <c r="V3" t="s">
-        <v>84</v>
-      </c>
-      <c r="W3" t="s">
-        <v>85</v>
-      </c>
-      <c r="X3" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>94</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>95</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>96</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>97</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>98</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>100</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>101</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>105</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>106</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>107</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>108</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>109</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>113</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>114</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>115</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>116</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>117</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>118</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>119</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>120</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:75">
+    <row r="4" spans="1:134">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="E4" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="F4" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="G4" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="H4" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="I4" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="J4" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="K4" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="L4" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="M4" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="N4" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="O4" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="P4" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="Q4" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="R4" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="S4" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="T4" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="U4" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="V4" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="W4" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="X4" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="Y4" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="Z4" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="AA4" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="AB4" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="AC4" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="AD4" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="AE4" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="AF4" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="AG4" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="AH4" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="AI4" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="AJ4" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="AK4" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="AL4" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="AM4" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="AN4" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="AO4" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="AP4" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="AQ4" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="AR4" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="AS4" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="AT4" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="AU4" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="AV4" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="AW4" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="AX4" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="AY4" t="s">
-        <v>170</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>171</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>172</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>173</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>174</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>175</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>176</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>177</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>178</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>179</v>
-      </c>
-      <c r="BI4" t="s">
-        <v>180</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>181</v>
-      </c>
-      <c r="BK4" t="s">
-        <v>182</v>
-      </c>
-      <c r="BL4" t="s">
-        <v>183</v>
-      </c>
-      <c r="BM4" t="s">
-        <v>184</v>
-      </c>
-      <c r="BN4" t="s">
-        <v>185</v>
-      </c>
-      <c r="BO4" t="s">
-        <v>186</v>
-      </c>
-      <c r="BP4" t="s">
-        <v>187</v>
-      </c>
-      <c r="BQ4" t="s">
-        <v>188</v>
-      </c>
-      <c r="BR4" t="s">
-        <v>189</v>
-      </c>
-      <c r="BS4" t="s">
-        <v>190</v>
-      </c>
-      <c r="BT4" t="s">
         <v>191</v>
       </c>
     </row>
@@ -1589,9 +1589,6 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
         <v>2</v>
       </c>
     </row>
@@ -1600,9 +1597,6 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
         <v>2</v>
       </c>
     </row>

</xml_diff>